<commit_message>
20220405 Build クラス Streamメソッド追加
</commit_message>
<xml_diff>
--- a/hulft.xlsx
+++ b/hulft.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="104">
   <si>
     <t xml:space="preserve">Index</t>
   </si>
@@ -132,6 +132,12 @@
     <t xml:space="preserve">C:\HULFT\LOOPSND2.txt</t>
   </si>
   <si>
+    <t xml:space="preserve">LOOPBACK3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C:\HULFT\LOOPSND3.txt</t>
+  </si>
+  <si>
     <t xml:space="preserve">RCVFILE</t>
   </si>
   <si>
@@ -204,6 +210,15 @@
     <t xml:space="preserve">RCV2</t>
   </si>
   <si>
+    <t xml:space="preserve">RCV2.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RCV3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RCV3.txt</t>
+  </si>
+  <si>
     <t xml:space="preserve">HOSTID</t>
   </si>
   <si>
@@ -288,6 +303,9 @@
     <t xml:space="preserve">Host2</t>
   </si>
   <si>
+    <t xml:space="preserve">Host3</t>
+  </si>
+  <si>
     <t xml:space="preserve">GRP</t>
   </si>
   <si>
@@ -310,6 +328,12 @@
   </si>
   <si>
     <t xml:space="preserve">  grp2host1,  grp2host2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRP3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">コメント3</t>
   </si>
 </sst>
 </file>
@@ -2567,6 +2591,56 @@
         <v>5</v>
       </c>
     </row>
+    <row r="6">
+      <c r="B6" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="M6" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="N6" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="O6" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="P6" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q6" s="27" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="B3:Q3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2614,7 +2688,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="44" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E3" s="44" t="s">
         <v>13</v>
@@ -2623,22 +2697,22 @@
         <v>14</v>
       </c>
       <c r="G3" s="44" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H3" s="44" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I3" s="44" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J3" s="44" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="K3" s="44" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="L3" s="44" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M3" s="44" t="s">
         <v>20</v>
@@ -2647,19 +2721,19 @@
         <v>21</v>
       </c>
       <c r="O3" s="44" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="P3" s="44" t="s">
         <v>19</v>
       </c>
       <c r="Q3" s="44" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="R3" s="44" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="S3" s="44" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4">
@@ -2667,55 +2741,55 @@
         <v>1</v>
       </c>
       <c r="C4" s="47" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D4" s="47" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E4" s="47" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F4" s="47" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G4" s="47" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H4" s="47" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I4" s="47" t="s">
         <v>30</v>
       </c>
       <c r="J4" s="47" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="K4" s="47" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="L4" s="47" t="s">
         <v>32</v>
       </c>
       <c r="M4" s="47" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="N4" s="47" t="s">
         <v>9</v>
       </c>
       <c r="O4" s="47" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="P4" s="47" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Q4" s="47" t="s">
         <v>32</v>
       </c>
       <c r="R4" s="47" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="S4" s="47" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5">
@@ -2723,55 +2797,111 @@
         <v>3</v>
       </c>
       <c r="C5" s="47" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D5" s="47" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E5" s="47" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F5" s="47" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="G5" s="47" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H5" s="47" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I5" s="47" t="s">
         <v>30</v>
       </c>
       <c r="J5" s="47" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="K5" s="47" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="L5" s="47" t="s">
         <v>32</v>
       </c>
       <c r="M5" s="47" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="N5" s="47" t="s">
         <v>9</v>
       </c>
       <c r="O5" s="47" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="P5" s="47" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Q5" s="47" t="s">
         <v>32</v>
       </c>
       <c r="R5" s="47" t="s">
+        <v>59</v>
+      </c>
+      <c r="S5" s="47" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="47" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="G6" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="H6" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="I6" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="K6" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="L6" s="47" t="s">
+        <v>32</v>
+      </c>
+      <c r="M6" s="47" t="s">
+        <v>56</v>
+      </c>
+      <c r="N6" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="O6" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="S5" s="47" t="s">
+      <c r="P6" s="47" t="s">
         <v>58</v>
+      </c>
+      <c r="Q6" s="47" t="s">
+        <v>32</v>
+      </c>
+      <c r="R6" s="47" t="s">
+        <v>59</v>
+      </c>
+      <c r="S6" s="47" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -2808,13 +2938,13 @@
         <v>19</v>
       </c>
       <c r="D3" s="84" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="E3" s="84" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="84" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4">
@@ -2822,16 +2952,16 @@
         <v>1</v>
       </c>
       <c r="C4" s="87" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D4" s="87" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="E4" s="87" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="F4" s="87" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5">
@@ -2839,16 +2969,33 @@
         <v>3</v>
       </c>
       <c r="C5" s="87" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D5" s="87" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="E5" s="87" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="F5" s="87" t="s">
-        <v>95</v>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="87" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="87" t="s">
+        <v>102</v>
+      </c>
+      <c r="E6" s="87" t="s">
+        <v>103</v>
+      </c>
+      <c r="F6" s="87" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2897,61 +3044,61 @@
         <v>10</v>
       </c>
       <c r="C3" s="64" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D3" s="64" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="E3" s="64" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="64" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="G3" s="64" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="H3" s="64" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="I3" s="64" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="J3" s="64" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="K3" s="64" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="L3" s="64" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="M3" s="64" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="N3" s="64" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="O3" s="64" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="P3" s="64" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="Q3" s="64" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="R3" s="64" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="S3" s="64" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="T3" s="64" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="U3" s="64" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4">
@@ -2962,58 +3109,58 @@
         <v>9</v>
       </c>
       <c r="D4" s="67" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E4" s="67" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F4" s="67" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="G4" s="67" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H4" s="67" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I4" s="67" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="J4" s="67" t="s">
         <v>9</v>
       </c>
       <c r="K4" s="67" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="L4" s="67" t="s">
         <v>32</v>
       </c>
       <c r="M4" s="67" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="N4" s="67" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="O4" s="67" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="P4" s="67" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="Q4" s="67" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="R4" s="67" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S4" s="67" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="T4" s="67" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="U4" s="67" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5">
@@ -3024,58 +3171,120 @@
         <v>9</v>
       </c>
       <c r="D5" s="67" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="67" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="67" t="s">
+        <v>84</v>
+      </c>
+      <c r="G5" s="67" t="s">
+        <v>85</v>
+      </c>
+      <c r="H5" s="67" t="s">
+        <v>86</v>
+      </c>
+      <c r="I5" s="67" t="s">
         <v>87</v>
-      </c>
-      <c r="E5" s="67" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="67" t="s">
-        <v>79</v>
-      </c>
-      <c r="G5" s="67" t="s">
-        <v>80</v>
-      </c>
-      <c r="H5" s="67" t="s">
-        <v>81</v>
-      </c>
-      <c r="I5" s="67" t="s">
-        <v>82</v>
       </c>
       <c r="J5" s="67" t="s">
         <v>9</v>
       </c>
       <c r="K5" s="67" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="L5" s="67" t="s">
         <v>32</v>
       </c>
       <c r="M5" s="67" t="s">
+        <v>89</v>
+      </c>
+      <c r="N5" s="67" t="s">
+        <v>90</v>
+      </c>
+      <c r="O5" s="67" t="s">
+        <v>91</v>
+      </c>
+      <c r="P5" s="67" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q5" s="67" t="s">
+        <v>89</v>
+      </c>
+      <c r="R5" s="67" t="s">
+        <v>89</v>
+      </c>
+      <c r="S5" s="67" t="s">
+        <v>89</v>
+      </c>
+      <c r="T5" s="67" t="s">
+        <v>89</v>
+      </c>
+      <c r="U5" s="67" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="67" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="67" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="67" t="s">
+        <v>93</v>
+      </c>
+      <c r="E6" s="67" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="67" t="s">
         <v>84</v>
       </c>
-      <c r="N5" s="67" t="s">
+      <c r="G6" s="67" t="s">
         <v>85</v>
       </c>
-      <c r="O5" s="67" t="s">
+      <c r="H6" s="67" t="s">
         <v>86</v>
       </c>
-      <c r="P5" s="67" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q5" s="67" t="s">
-        <v>84</v>
-      </c>
-      <c r="R5" s="67" t="s">
-        <v>84</v>
-      </c>
-      <c r="S5" s="67" t="s">
-        <v>84</v>
-      </c>
-      <c r="T5" s="67" t="s">
-        <v>84</v>
-      </c>
-      <c r="U5" s="67" t="s">
-        <v>84</v>
+      <c r="I6" s="67" t="s">
+        <v>87</v>
+      </c>
+      <c r="J6" s="67" t="s">
+        <v>9</v>
+      </c>
+      <c r="K6" s="67" t="s">
+        <v>88</v>
+      </c>
+      <c r="L6" s="67" t="s">
+        <v>32</v>
+      </c>
+      <c r="M6" s="67" t="s">
+        <v>89</v>
+      </c>
+      <c r="N6" s="67" t="s">
+        <v>90</v>
+      </c>
+      <c r="O6" s="67" t="s">
+        <v>91</v>
+      </c>
+      <c r="P6" s="67" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q6" s="67" t="s">
+        <v>89</v>
+      </c>
+      <c r="R6" s="67" t="s">
+        <v>89</v>
+      </c>
+      <c r="S6" s="67" t="s">
+        <v>89</v>
+      </c>
+      <c r="T6" s="67" t="s">
+        <v>89</v>
+      </c>
+      <c r="U6" s="67" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>